<commit_message>
refactor: implemented color, positon, abstractions
</commit_message>
<xml_diff>
--- a/matrizen.xlsx
+++ b/matrizen.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\CSharp\LostInLabyrinth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65A41CB3-998A-4C31-8B2A-5D3C2B9CC70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0695B7-79D9-421F-BF1A-46F39DED3DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0F759D0A-00A9-436F-A92D-FA78A0E6C1F4}"/>
+    <workbookView xWindow="6105" yWindow="4605" windowWidth="21600" windowHeight="10530" xr2:uid="{0F759D0A-00A9-436F-A92D-FA78A0E6C1F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Matritzen" sheetId="1" r:id="rId1"/>
-    <sheet name="Orthographic " sheetId="2" r:id="rId2"/>
+    <sheet name="Inverse" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="109">
   <si>
     <t>a</t>
   </si>
@@ -82,9 +83,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>3 * Y</t>
-  </si>
-  <si>
     <t>3 * x</t>
   </si>
   <si>
@@ -329,6 +327,33 @@
   </si>
   <si>
     <t>-5/6</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>4* Y</t>
+  </si>
+  <si>
+    <t>1/640</t>
+  </si>
+  <si>
+    <t>1/390</t>
+  </si>
+  <si>
+    <t>-1/640</t>
+  </si>
+  <si>
+    <t>-1/390</t>
+  </si>
+  <si>
+    <t>A^T = B</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>(A*B)^T=B^T * A ^T</t>
   </si>
 </sst>
 </file>
@@ -541,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -660,6 +685,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -976,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CFC77B-DA5C-463B-A681-BC86DEFC14D5}">
   <dimension ref="A1:AM21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AH15" sqref="AH15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,16 +1041,16 @@
   <sheetData>
     <row r="1" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" t="s">
         <v>26</v>
       </c>
-      <c r="T1" t="s">
-        <v>27</v>
-      </c>
       <c r="AB1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
@@ -1073,10 +1100,10 @@
         <v>4</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="U2" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V2" s="7">
         <v>0</v>
@@ -1091,7 +1118,7 @@
         <v>10</v>
       </c>
       <c r="Z2" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AB2" s="6">
         <v>1</v>
@@ -1106,10 +1133,10 @@
         <v>5</v>
       </c>
       <c r="AF2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG2" s="22" t="s">
         <v>34</v>
-      </c>
-      <c r="AG2" s="22" t="s">
-        <v>35</v>
       </c>
       <c r="AH2" s="7">
         <v>0</v>
@@ -1118,10 +1145,10 @@
         <v>10</v>
       </c>
       <c r="AJ2" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AK2" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AL2" s="25" t="s">
         <v>1</v>
@@ -1162,10 +1189,10 @@
         <v>17</v>
       </c>
       <c r="T3" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="U3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="V3" s="15">
         <v>0</v>
@@ -1174,7 +1201,7 @@
         <v>17</v>
       </c>
       <c r="Z3" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AB3" s="14">
         <v>0</v>
@@ -1186,19 +1213,19 @@
         <v>2</v>
       </c>
       <c r="AF3" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AG3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AH3" s="15">
         <v>0</v>
       </c>
       <c r="AJ3" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AK3" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AL3" s="28" t="s">
         <v>2</v>
@@ -1315,19 +1342,19 @@
         <v>10</v>
       </c>
       <c r="P6" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="R6" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AB6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC6" s="22" t="s">
         <v>34</v>
-      </c>
-      <c r="AC6" s="22" t="s">
-        <v>35</v>
       </c>
       <c r="AD6" s="7">
         <v>0</v>
@@ -1348,13 +1375,13 @@
         <v>10</v>
       </c>
       <c r="AJ6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK6" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="AK6" s="22" t="s">
-        <v>35</v>
-      </c>
       <c r="AL6" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1371,16 +1398,16 @@
         <v>17</v>
       </c>
       <c r="P7" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R7" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AB7" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AC7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD7" s="15">
         <v>0</v>
@@ -1395,13 +1422,13 @@
         <v>2</v>
       </c>
       <c r="AJ7" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AK7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AL7" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1436,7 +1463,7 @@
         <v>1</v>
       </c>
       <c r="P8" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R8" s="21">
         <v>1</v>
@@ -1501,13 +1528,13 @@
         <v>10</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AA11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB11" s="22" t="s">
         <v>40</v>
-      </c>
-      <c r="AB11" s="22" t="s">
-        <v>41</v>
       </c>
       <c r="AC11" s="7">
         <v>60</v>
@@ -1516,7 +1543,7 @@
         <v>0.5</v>
       </c>
       <c r="AK11" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AL11" s="7">
         <v>-1.964</v>
@@ -1527,19 +1554,19 @@
         <v>0</v>
       </c>
       <c r="B12" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>18</v>
+        <v>101</v>
       </c>
       <c r="AA12" s="14" t="s">
         <v>1</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC12" s="15">
         <v>3</v>
@@ -1574,36 +1601,95 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="36:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="36:39" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A15" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A16" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A18" s="54"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
       <c r="AJ18" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK18" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="AK18" s="22" t="s">
+      <c r="AL18" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM18" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A19" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="55" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ19" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="AL18" s="16" t="s">
+      <c r="AK19" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL19" t="s">
         <v>37</v>
       </c>
-      <c r="AM18" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="36:39" x14ac:dyDescent="0.25">
-      <c r="AJ19" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK19" t="s">
-        <v>34</v>
-      </c>
-      <c r="AL19" t="s">
-        <v>38</v>
-      </c>
       <c r="AM19" s="15">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="36:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A20" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" t="s">
+        <v>108</v>
+      </c>
       <c r="AJ20" s="14">
         <v>0</v>
       </c>
@@ -1617,7 +1703,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="36:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>107</v>
+      </c>
       <c r="AJ21" s="8">
         <v>0</v>
       </c>
@@ -1640,7 +1735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD11FB64-53B4-4ADE-A562-1C2E020B905D}">
   <dimension ref="A3:AB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA21" sqref="AA21"/>
     </sheetView>
   </sheetViews>
@@ -1670,7 +1765,7 @@
     <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="G4" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H4" s="33">
         <v>1</v>
@@ -1682,7 +1777,7 @@
         <v>5</v>
       </c>
       <c r="M4" s="37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N4" s="33" t="s">
         <v>5</v>
@@ -1703,18 +1798,18 @@
         <v>0</v>
       </c>
       <c r="U4" s="35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="X4" s="35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA4" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="34" t="s">
         <v>10</v>
@@ -1723,7 +1818,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="34"/>
       <c r="H5" s="33">
@@ -1736,7 +1831,7 @@
         <v>4</v>
       </c>
       <c r="M5" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O5" s="38" t="s">
         <v>2</v>
@@ -1751,13 +1846,13 @@
         <v>1</v>
       </c>
       <c r="U5" s="35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="X5" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AA5" s="33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -1765,33 +1860,33 @@
         <v>4</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="U6" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="X6" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AA6" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB6" s="33" t="s">
         <v>92</v>
-      </c>
-      <c r="AB6" s="33" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="U7" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X7" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AA7" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AB7" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -1799,7 +1894,7 @@
         <v>5</v>
       </c>
       <c r="M8" s="37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N8" s="33" t="s">
         <v>5</v>
@@ -1814,33 +1909,33 @@
         <v>10</v>
       </c>
       <c r="R8" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="S8" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="S8" s="47" t="s">
-        <v>51</v>
-      </c>
       <c r="X8" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y8" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="Y8" s="33" t="s">
-        <v>72</v>
-      </c>
       <c r="AA8" s="33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H9" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J9" s="33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L9" s="38">
         <v>4</v>
       </c>
       <c r="M9" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O9" s="38" t="s">
         <v>2</v>
@@ -1849,41 +1944,41 @@
         <v>3</v>
       </c>
       <c r="R9" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="S9" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="S9" s="49" t="s">
-        <v>53</v>
-      </c>
       <c r="U9" s="35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="X9" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y9" s="33" t="s">
         <v>73</v>
-      </c>
-      <c r="Y9" s="33" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="H10" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U10" s="35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X10" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA10" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="U11" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AA11" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -1891,16 +1986,16 @@
         <v>5</v>
       </c>
       <c r="M12" s="37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N12" s="33" t="s">
         <v>5</v>
       </c>
       <c r="O12" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P12" s="41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q12" s="34" t="s">
         <v>10</v>
@@ -1912,13 +2007,13 @@
         <v>0</v>
       </c>
       <c r="U12" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="X12" s="34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AA12" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1926,13 +2021,13 @@
         <v>4</v>
       </c>
       <c r="M13" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O13" s="42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P13" s="43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R13" s="52">
         <v>0</v>
@@ -1941,114 +2036,340 @@
         <v>1</v>
       </c>
       <c r="X13" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AA13" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="U14" s="35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="X14" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="U15" s="35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="X16" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="21:25" x14ac:dyDescent="0.25">
       <c r="U17" s="35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V17" s="33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="X17" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="21:25" x14ac:dyDescent="0.25">
       <c r="U18" s="34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="21:25" x14ac:dyDescent="0.25">
       <c r="U19" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="V19" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="V19" s="33" t="s">
-        <v>65</v>
-      </c>
       <c r="X19" s="34" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Y19" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="21:25" x14ac:dyDescent="0.25">
       <c r="U20" s="34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="X20" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y20" s="33" t="s">
         <v>79</v>
-      </c>
-      <c r="Y20" s="33" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="21" spans="21:25" x14ac:dyDescent="0.25">
       <c r="U21" s="34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="X21" s="34" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="21:25" x14ac:dyDescent="0.25">
       <c r="X22" s="33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="21:25" x14ac:dyDescent="0.25">
       <c r="X23" s="33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="21:25" x14ac:dyDescent="0.25">
       <c r="X24" s="33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Y24" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="21:25" x14ac:dyDescent="0.25">
       <c r="X25" s="33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="21:25" x14ac:dyDescent="0.25">
       <c r="X26" s="33" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="21:25" x14ac:dyDescent="0.25">
       <c r="X27" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{233F45F5-A465-4FED-B528-610F433A716C}">
+  <dimension ref="A3:L16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="33">
+        <v>0</v>
+      </c>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="33">
+        <v>0</v>
+      </c>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>-1</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" t="s">
+        <v>102</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>-1</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
+        <v>103</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>